<commit_message>
Actualizaci├│n completa de ProFru
</commit_message>
<xml_diff>
--- a/data/ProFru.xlsx
+++ b/data/ProFru.xlsx
@@ -26968,11 +26968,11 @@
         </is>
       </c>
       <c r="E522" s="0">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="F522" s="0" t="inlineStr">
         <is>
-          <t>GLOBAL FRESH</t>
+          <t>MOÑO AZUL SA</t>
         </is>
       </c>
       <c r="G522" s="0" t="inlineStr">
@@ -34834,11 +34834,11 @@
         </is>
       </c>
       <c r="E676" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F676" s="0" t="inlineStr">
         <is>
-          <t>MOÑO AZUL SA</t>
+          <t>CONTADINI SRL</t>
         </is>
       </c>
       <c r="G676" s="0" t="inlineStr">
@@ -34857,14 +34857,14 @@
         </is>
       </c>
       <c r="J676" s="0">
-        <v>6992</v>
+        <v>7440</v>
       </c>
       <c r="K676" s="0"/>
       <c r="L676" s="0">
         <v>0</v>
       </c>
       <c r="M676" s="0">
-        <v>6992</v>
+        <v>7440</v>
       </c>
     </row>
     <row outlineLevel="0" r="677">
@@ -35756,7 +35756,7 @@
       </c>
       <c r="F694" s="0" t="inlineStr">
         <is>
-          <t>CIFUENTES MARCELO</t>
+          <t>MINISINI JORGE RAUL</t>
         </is>
       </c>
       <c r="G694" s="0" t="inlineStr">
@@ -38341,11 +38341,11 @@
         </is>
       </c>
       <c r="E745" s="0">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F745" s="0" t="inlineStr">
         <is>
-          <t>MINISINI JORGE RAUL</t>
+          <t>ANDAGRI</t>
         </is>
       </c>
       <c r="G745" s="0" t="inlineStr">
@@ -38364,14 +38364,14 @@
         </is>
       </c>
       <c r="J745" s="0">
-        <v>8081.65</v>
+        <v>13840</v>
       </c>
       <c r="K745" s="0"/>
       <c r="L745" s="0">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M745" s="0">
-        <v>8507</v>
+        <v>13840</v>
       </c>
     </row>
     <row outlineLevel="0" r="746">

</xml_diff>